<commit_message>
TEST CASES FILE COMPLETE AND READY TO EXECUTE TEST CASES
</commit_message>
<xml_diff>
--- a/04Test Cases Design/Test_cases.xlsx
+++ b/04Test Cases Design/Test_cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\SOFTWARE TESTING\TESTING PROJECTS\Opencart.demo testing project\04Test Cases Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDFA490C-23E5-4AC4-8F41-015F04DBC0B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{934CEE0C-429F-4073-9958-E0C4A644A6CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="245">
   <si>
     <t>TC_ID</t>
   </si>
@@ -836,12 +836,72 @@
     <t>1.Add product to cart.
 2.Refresh browser page.</t>
   </si>
+  <si>
+    <t>First Name: Rahul
+Last Name: Sharma
+Email: rahul.test01@gmail.com
+Telephone: 9876543210
+Password: Test@123
+Confirm: Test@123</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Email: onlymail@test.com
+Password: Test@123</t>
+  </si>
+  <si>
+    <t>rahul123gmail.com</t>
+  </si>
+  <si>
+    <t>Password: Test@123
+Confirm: Test@999</t>
+  </si>
+  <si>
+    <t>rahul.test01@gmail.com
+ / Test12300</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NA
+</t>
+  </si>
+  <si>
+    <t>mac, iphone, camera</t>
+  </si>
+  <si>
+    <t>Select category “Laptops &amp; Notebooks”</t>
+  </si>
+  <si>
+    <t>macbook with retina display</t>
+  </si>
+  <si>
+    <t>mac, laptop, apple</t>
+  </si>
+  <si>
+    <t>asdfgh123</t>
+  </si>
+  <si>
+    <t>"@#$%"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rahul.test01@gmail.com
+</t>
+  </si>
+  <si>
+    <t>USERNAME:rahul.test01@gmail.com
+PASS: Test@123</t>
+  </si>
+  <si>
+    <t>USERNAME:rahul1@gmail.com
+ PASS: Test@123878</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -863,6 +923,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -906,10 +974,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -926,8 +995,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1208,25 +1281,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView tabSelected="1" topLeftCell="D7" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="54.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.28515625" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.28515625" customWidth="1"/>
+    <col min="6" max="6" width="54.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33.28515625" customWidth="1"/>
     <col min="8" max="8" width="64.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18.75">
+    <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1234,16 +1307,16 @@
         <v>119</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>129</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>116</v>
@@ -1258,7 +1331,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="75">
+    <row r="2" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
@@ -1266,25 +1339,27 @@
         <v>182</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="G2" s="4"/>
+      <c r="G2" s="5" t="s">
+        <v>229</v>
+      </c>
       <c r="H2" s="5" t="s">
         <v>141</v>
       </c>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
     </row>
-    <row r="3" spans="1:10" ht="30">
+    <row r="3" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -1292,25 +1367,27 @@
         <v>182</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="G3" s="4"/>
+      <c r="G3" s="4" t="s">
+        <v>230</v>
+      </c>
       <c r="H3" s="4" t="s">
         <v>142</v>
       </c>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
     </row>
-    <row r="4" spans="1:10" ht="60">
+    <row r="4" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
@@ -1318,25 +1395,27 @@
         <v>182</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="G4" s="4"/>
+      <c r="G4" s="4" t="s">
+        <v>230</v>
+      </c>
       <c r="H4" s="4" t="s">
         <v>143</v>
       </c>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
     </row>
-    <row r="5" spans="1:10" ht="75">
+    <row r="5" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>10</v>
       </c>
@@ -1344,25 +1423,27 @@
         <v>182</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="F5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>197</v>
-      </c>
-      <c r="G5" s="4"/>
+      <c r="G5" s="4" t="s">
+        <v>230</v>
+      </c>
       <c r="H5" s="4" t="s">
         <v>144</v>
       </c>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
     </row>
-    <row r="6" spans="1:10" ht="60">
+    <row r="6" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>12</v>
       </c>
@@ -1370,25 +1451,27 @@
         <v>182</v>
       </c>
       <c r="C6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="G6" s="4"/>
+      <c r="G6" s="5" t="s">
+        <v>231</v>
+      </c>
       <c r="H6" s="4" t="s">
         <v>145</v>
       </c>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
     </row>
-    <row r="7" spans="1:10" ht="45">
+    <row r="7" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>14</v>
       </c>
@@ -1396,25 +1479,27 @@
         <v>182</v>
       </c>
       <c r="C7" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="F7" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>199</v>
-      </c>
-      <c r="G7" s="4"/>
+      <c r="G7" s="4" t="s">
+        <v>230</v>
+      </c>
       <c r="H7" s="4" t="s">
         <v>146</v>
       </c>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
     </row>
-    <row r="8" spans="1:10" ht="45">
+    <row r="8" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>16</v>
       </c>
@@ -1422,16 +1507,16 @@
         <v>182</v>
       </c>
       <c r="C8" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>17</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>200</v>
       </c>
       <c r="G8" s="4"/>
       <c r="H8" s="4" t="s">
@@ -1440,7 +1525,7 @@
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
     </row>
-    <row r="9" spans="1:10" ht="60">
+    <row r="9" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>18</v>
       </c>
@@ -1448,25 +1533,27 @@
         <v>182</v>
       </c>
       <c r="C9" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="F9" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>201</v>
-      </c>
-      <c r="G9" s="4"/>
+      <c r="G9" s="6" t="s">
+        <v>242</v>
+      </c>
       <c r="H9" s="4" t="s">
         <v>148</v>
       </c>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
     </row>
-    <row r="10" spans="1:10" ht="45">
+    <row r="10" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>20</v>
       </c>
@@ -1474,25 +1561,27 @@
         <v>182</v>
       </c>
       <c r="C10" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="F10" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>202</v>
-      </c>
-      <c r="G10" s="4"/>
+      <c r="G10" s="4" t="s">
+        <v>232</v>
+      </c>
       <c r="H10" s="4" t="s">
         <v>149</v>
       </c>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
     </row>
-    <row r="11" spans="1:10" ht="45">
+    <row r="11" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>22</v>
       </c>
@@ -1500,25 +1589,27 @@
         <v>182</v>
       </c>
       <c r="C11" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="F11" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>203</v>
-      </c>
-      <c r="G11" s="4"/>
+      <c r="G11" s="5" t="s">
+        <v>233</v>
+      </c>
       <c r="H11" t="s">
         <v>150</v>
       </c>
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
     </row>
-    <row r="12" spans="1:10" ht="60">
+    <row r="12" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>24</v>
       </c>
@@ -1526,25 +1617,27 @@
         <v>182</v>
       </c>
       <c r="C12" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="F12" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>204</v>
-      </c>
-      <c r="G12" s="4"/>
+      <c r="G12" s="4" t="s">
+        <v>230</v>
+      </c>
       <c r="H12" s="4" t="s">
         <v>151</v>
       </c>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
     </row>
-    <row r="13" spans="1:10" ht="45">
+    <row r="13" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>26</v>
       </c>
@@ -1552,25 +1645,27 @@
         <v>183</v>
       </c>
       <c r="C13" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="F13" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="G13" s="4"/>
+      <c r="G13" s="5" t="s">
+        <v>243</v>
+      </c>
       <c r="H13" s="4" t="s">
         <v>152</v>
       </c>
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
     </row>
-    <row r="14" spans="1:10" ht="45">
+    <row r="14" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>29</v>
       </c>
@@ -1578,25 +1673,27 @@
         <v>184</v>
       </c>
       <c r="C14" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="F14" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D14" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>209</v>
-      </c>
-      <c r="G14" s="4"/>
+      <c r="G14" s="5" t="s">
+        <v>244</v>
+      </c>
       <c r="H14" s="4" t="s">
         <v>153</v>
       </c>
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
     </row>
-    <row r="15" spans="1:10" ht="45">
+    <row r="15" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>31</v>
       </c>
@@ -1604,25 +1701,27 @@
         <v>184</v>
       </c>
       <c r="C15" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="F15" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="G15" s="4"/>
+      <c r="G15" s="6" t="s">
+        <v>234</v>
+      </c>
       <c r="H15" t="s">
         <v>153</v>
       </c>
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
     </row>
-    <row r="16" spans="1:10" ht="45">
+    <row r="16" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>33</v>
       </c>
@@ -1630,25 +1729,27 @@
         <v>184</v>
       </c>
       <c r="C16" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="F16" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D16" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>211</v>
-      </c>
-      <c r="G16" s="4"/>
+      <c r="G16" s="1" t="s">
+        <v>235</v>
+      </c>
       <c r="H16" t="s">
         <v>154</v>
       </c>
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
     </row>
-    <row r="17" spans="1:10" ht="45">
+    <row r="17" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>35</v>
       </c>
@@ -1656,25 +1757,27 @@
         <v>184</v>
       </c>
       <c r="C17" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="F17" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D17" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="G17" s="4"/>
+      <c r="G17" s="4" t="s">
+        <v>230</v>
+      </c>
       <c r="H17" t="s">
         <v>154</v>
       </c>
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
     </row>
-    <row r="18" spans="1:10" ht="30">
+    <row r="18" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>37</v>
       </c>
@@ -1682,94 +1785,102 @@
         <v>184</v>
       </c>
       <c r="C18" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="F18" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D18" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="G18" s="4"/>
+      <c r="G18" s="4" t="s">
+        <v>230</v>
+      </c>
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
     </row>
-    <row r="19" spans="1:10" ht="45">
+    <row r="19" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>39</v>
       </c>
       <c r="B19" s="4"/>
       <c r="C19" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="F19" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D19" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="G19" s="4"/>
+      <c r="G19" s="4" t="s">
+        <v>230</v>
+      </c>
       <c r="H19" t="s">
         <v>155</v>
       </c>
       <c r="I19" s="4"/>
       <c r="J19" s="4"/>
     </row>
-    <row r="20" spans="1:10" ht="30">
+    <row r="20" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>41</v>
       </c>
       <c r="B20" s="4"/>
       <c r="C20" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="F20" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D20" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="G20" s="4"/>
+      <c r="G20" s="4" t="s">
+        <v>230</v>
+      </c>
       <c r="H20" s="4" t="s">
         <v>156</v>
       </c>
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
     </row>
-    <row r="21" spans="1:10" ht="30">
+    <row r="21" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>43</v>
       </c>
       <c r="B21" s="4"/>
       <c r="C21" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="F21" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D21" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="G21" s="4"/>
+      <c r="G21" s="4" t="s">
+        <v>230</v>
+      </c>
       <c r="H21" t="s">
         <v>157</v>
       </c>
       <c r="I21" s="4"/>
       <c r="J21" s="4"/>
     </row>
-    <row r="22" spans="1:10" ht="45">
+    <row r="22" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>45</v>
       </c>
@@ -1777,25 +1888,27 @@
         <v>185</v>
       </c>
       <c r="C22" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="F22" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D22" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="G22" s="4"/>
+      <c r="G22" s="4" t="s">
+        <v>236</v>
+      </c>
       <c r="H22" t="s">
         <v>158</v>
       </c>
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
     </row>
-    <row r="23" spans="1:10" ht="60">
+    <row r="23" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>48</v>
       </c>
@@ -1803,25 +1916,27 @@
         <v>185</v>
       </c>
       <c r="C23" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="F23" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D23" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="G23" s="4"/>
+      <c r="G23" s="4" t="s">
+        <v>237</v>
+      </c>
       <c r="H23" t="s">
         <v>159</v>
       </c>
       <c r="I23" s="4"/>
       <c r="J23" s="4"/>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>50</v>
       </c>
@@ -1829,25 +1944,27 @@
         <v>185</v>
       </c>
       <c r="C24" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="F24" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D24" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="G24" s="4"/>
+      <c r="G24" s="4" t="s">
+        <v>238</v>
+      </c>
       <c r="H24" t="s">
         <v>160</v>
       </c>
       <c r="I24" s="4"/>
       <c r="J24" s="4"/>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>52</v>
       </c>
@@ -1855,25 +1972,27 @@
         <v>185</v>
       </c>
       <c r="C25" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="E25" t="s">
+        <v>137</v>
+      </c>
+      <c r="F25" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="D25" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="F25" t="s">
-        <v>137</v>
-      </c>
-      <c r="G25" s="4"/>
+      <c r="G25" s="4" t="s">
+        <v>239</v>
+      </c>
       <c r="H25" s="4" t="s">
         <v>160</v>
       </c>
       <c r="I25" s="4"/>
       <c r="J25" s="4"/>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>54</v>
       </c>
@@ -1881,25 +2000,27 @@
         <v>185</v>
       </c>
       <c r="C26" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="E26" t="s">
+        <v>138</v>
+      </c>
+      <c r="F26" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D26" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="F26" t="s">
-        <v>138</v>
-      </c>
-      <c r="G26" s="4"/>
+      <c r="G26" s="4" t="s">
+        <v>230</v>
+      </c>
       <c r="H26" t="s">
         <v>161</v>
       </c>
       <c r="I26" s="4"/>
       <c r="J26" s="4"/>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>56</v>
       </c>
@@ -1907,25 +2028,27 @@
         <v>185</v>
       </c>
       <c r="C27" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="E27" t="s">
+        <v>139</v>
+      </c>
+      <c r="F27" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="D27" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="F27" t="s">
-        <v>139</v>
-      </c>
-      <c r="G27" s="4"/>
+      <c r="G27" s="4" t="s">
+        <v>240</v>
+      </c>
       <c r="H27" t="s">
         <v>162</v>
       </c>
       <c r="I27" s="4"/>
       <c r="J27" s="4"/>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>58</v>
       </c>
@@ -1933,25 +2056,27 @@
         <v>185</v>
       </c>
       <c r="C28" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="E28" t="s">
+        <v>140</v>
+      </c>
+      <c r="F28" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="D28" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="F28" t="s">
-        <v>140</v>
-      </c>
-      <c r="G28" s="4"/>
+      <c r="G28" s="4" t="s">
+        <v>241</v>
+      </c>
       <c r="H28" t="s">
         <v>163</v>
       </c>
       <c r="I28" s="4"/>
       <c r="J28" s="4"/>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>60</v>
       </c>
@@ -1959,25 +2084,27 @@
         <v>186</v>
       </c>
       <c r="C29" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="F29" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="D29" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="E29" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="G29" s="4"/>
+      <c r="G29" s="4" t="s">
+        <v>230</v>
+      </c>
       <c r="H29" t="s">
         <v>164</v>
       </c>
       <c r="I29" s="4"/>
       <c r="J29" s="4"/>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>63</v>
       </c>
@@ -1985,25 +2112,27 @@
         <v>186</v>
       </c>
       <c r="C30" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="F30" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D30" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="E30" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="G30" s="4"/>
+      <c r="G30" s="4" t="s">
+        <v>230</v>
+      </c>
       <c r="H30" t="s">
         <v>164</v>
       </c>
       <c r="I30" s="4"/>
       <c r="J30" s="4"/>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>65</v>
       </c>
@@ -2011,25 +2140,27 @@
         <v>186</v>
       </c>
       <c r="C31" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="F31" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="D31" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="E31" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="G31" s="4"/>
+      <c r="G31" s="4" t="s">
+        <v>230</v>
+      </c>
       <c r="H31" t="s">
         <v>164</v>
       </c>
       <c r="I31" s="4"/>
       <c r="J31" s="4"/>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>67</v>
       </c>
@@ -2037,25 +2168,27 @@
         <v>186</v>
       </c>
       <c r="C32" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="F32" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="D32" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="E32" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="F32" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="G32" s="4"/>
+      <c r="G32" s="4" t="s">
+        <v>230</v>
+      </c>
       <c r="H32" t="s">
         <v>164</v>
       </c>
       <c r="I32" s="4"/>
       <c r="J32" s="4"/>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>69</v>
       </c>
@@ -2063,25 +2196,27 @@
         <v>186</v>
       </c>
       <c r="C33" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="F33" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="D33" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="E33" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="F33" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="G33" s="4"/>
+      <c r="G33" s="4" t="s">
+        <v>230</v>
+      </c>
       <c r="H33" t="s">
         <v>164</v>
       </c>
       <c r="I33" s="4"/>
       <c r="J33" s="4"/>
     </row>
-    <row r="34" spans="1:10" ht="105">
+    <row r="34" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>71</v>
       </c>
@@ -2089,25 +2224,27 @@
         <v>187</v>
       </c>
       <c r="C34" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="F34" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="D34" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="E34" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="F34" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G34" s="4"/>
+      <c r="G34" s="4" t="s">
+        <v>230</v>
+      </c>
       <c r="H34" t="s">
         <v>165</v>
       </c>
       <c r="I34" s="4"/>
       <c r="J34" s="4"/>
     </row>
-    <row r="35" spans="1:10" ht="45">
+    <row r="35" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>73</v>
       </c>
@@ -2115,25 +2252,27 @@
         <v>187</v>
       </c>
       <c r="C35" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="F35" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="D35" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="E35" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="F35" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="G35" s="4"/>
+      <c r="G35" s="4" t="s">
+        <v>230</v>
+      </c>
       <c r="H35" t="s">
         <v>166</v>
       </c>
       <c r="I35" s="4"/>
       <c r="J35" s="4"/>
     </row>
-    <row r="36" spans="1:10" ht="45">
+    <row r="36" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>76</v>
       </c>
@@ -2141,25 +2280,27 @@
         <v>189</v>
       </c>
       <c r="C36" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="F36" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="D36" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="E36" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="F36" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="G36" s="4"/>
+      <c r="G36" s="4" t="s">
+        <v>230</v>
+      </c>
       <c r="H36" t="s">
         <v>167</v>
       </c>
       <c r="I36" s="4"/>
       <c r="J36" s="4"/>
     </row>
-    <row r="37" spans="1:10" ht="60">
+    <row r="37" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>78</v>
       </c>
@@ -2167,25 +2308,27 @@
         <v>188</v>
       </c>
       <c r="C37" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="F37" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="D37" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="E37" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="F37" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="G37" s="4"/>
+      <c r="G37" s="4" t="s">
+        <v>230</v>
+      </c>
       <c r="H37" t="s">
         <v>168</v>
       </c>
       <c r="I37" s="4"/>
       <c r="J37" s="4"/>
     </row>
-    <row r="38" spans="1:10" ht="60">
+    <row r="38" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>80</v>
       </c>
@@ -2193,25 +2336,27 @@
         <v>188</v>
       </c>
       <c r="C38" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="F38" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="D38" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="E38" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="F38" s="5" t="s">
-        <v>219</v>
-      </c>
-      <c r="G38" s="4"/>
+      <c r="G38" s="4" t="s">
+        <v>230</v>
+      </c>
       <c r="H38" t="s">
         <v>168</v>
       </c>
       <c r="I38" s="4"/>
       <c r="J38" s="4"/>
     </row>
-    <row r="39" spans="1:10" ht="30">
+    <row r="39" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>82</v>
       </c>
@@ -2219,25 +2364,27 @@
         <v>188</v>
       </c>
       <c r="C39" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="F39" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="D39" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="E39" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="F39" s="5" t="s">
-        <v>228</v>
-      </c>
-      <c r="G39" s="4"/>
+      <c r="G39" s="4" t="s">
+        <v>230</v>
+      </c>
       <c r="H39" t="s">
         <v>169</v>
       </c>
       <c r="I39" s="4"/>
       <c r="J39" s="4"/>
     </row>
-    <row r="40" spans="1:10" ht="45">
+    <row r="40" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>84</v>
       </c>
@@ -2245,25 +2392,27 @@
         <v>188</v>
       </c>
       <c r="C40" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="F40" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="D40" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="E40" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="F40" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="G40" s="4"/>
+      <c r="G40" s="4" t="s">
+        <v>230</v>
+      </c>
       <c r="H40" t="s">
         <v>170</v>
       </c>
       <c r="I40" s="4"/>
       <c r="J40" s="4"/>
     </row>
-    <row r="41" spans="1:10" ht="45">
+    <row r="41" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>86</v>
       </c>
@@ -2271,25 +2420,27 @@
         <v>190</v>
       </c>
       <c r="C41" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="F41" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="D41" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="E41" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="F41" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="G41" s="4"/>
+      <c r="G41" s="4" t="s">
+        <v>230</v>
+      </c>
       <c r="H41" t="s">
         <v>171</v>
       </c>
       <c r="I41" s="4"/>
       <c r="J41" s="4"/>
     </row>
-    <row r="42" spans="1:10" ht="105">
+    <row r="42" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>89</v>
       </c>
@@ -2297,25 +2448,27 @@
         <v>191</v>
       </c>
       <c r="C42" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="F42" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="D42" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="E42" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="F42" s="5" t="s">
-        <v>221</v>
-      </c>
-      <c r="G42" s="4"/>
+      <c r="G42" s="4" t="s">
+        <v>230</v>
+      </c>
       <c r="H42" t="s">
         <v>172</v>
       </c>
       <c r="I42" s="4"/>
       <c r="J42" s="4"/>
     </row>
-    <row r="43" spans="1:10" ht="45">
+    <row r="43" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>91</v>
       </c>
@@ -2323,25 +2476,27 @@
         <v>191</v>
       </c>
       <c r="C43" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="F43" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="D43" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="E43" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="F43" s="5" t="s">
-        <v>222</v>
-      </c>
-      <c r="G43" s="4"/>
+      <c r="G43" s="4" t="s">
+        <v>230</v>
+      </c>
       <c r="H43" t="s">
         <v>173</v>
       </c>
       <c r="I43" s="4"/>
       <c r="J43" s="4"/>
     </row>
-    <row r="44" spans="1:10" ht="60">
+    <row r="44" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>93</v>
       </c>
@@ -2349,25 +2504,27 @@
         <v>191</v>
       </c>
       <c r="C44" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="F44" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="D44" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="E44" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="F44" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="G44" s="4"/>
+      <c r="G44" s="4" t="s">
+        <v>230</v>
+      </c>
       <c r="H44" t="s">
         <v>174</v>
       </c>
       <c r="I44" s="4"/>
       <c r="J44" s="4"/>
     </row>
-    <row r="45" spans="1:10" ht="60">
+    <row r="45" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>95</v>
       </c>
@@ -2375,25 +2532,27 @@
         <v>191</v>
       </c>
       <c r="C45" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="F45" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="D45" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="E45" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="F45" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="G45" s="4"/>
+      <c r="G45" s="4" t="s">
+        <v>230</v>
+      </c>
       <c r="H45" t="s">
         <v>174</v>
       </c>
       <c r="I45" s="4"/>
       <c r="J45" s="4"/>
     </row>
-    <row r="46" spans="1:10" ht="30">
+    <row r="46" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>97</v>
       </c>
@@ -2401,25 +2560,27 @@
         <v>192</v>
       </c>
       <c r="C46" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="F46" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="D46" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="E46" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="F46" s="5" t="s">
-        <v>227</v>
-      </c>
-      <c r="G46" s="4"/>
+      <c r="G46" s="4" t="s">
+        <v>230</v>
+      </c>
       <c r="H46" t="s">
         <v>175</v>
       </c>
       <c r="I46" s="4"/>
       <c r="J46" s="4"/>
     </row>
-    <row r="47" spans="1:10" ht="60">
+    <row r="47" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>100</v>
       </c>
@@ -2427,25 +2588,27 @@
         <v>192</v>
       </c>
       <c r="C47" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="F47" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="D47" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="E47" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="F47" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="G47" s="4"/>
+      <c r="G47" s="4" t="s">
+        <v>230</v>
+      </c>
       <c r="H47" t="s">
         <v>175</v>
       </c>
       <c r="I47" s="4"/>
       <c r="J47" s="4"/>
     </row>
-    <row r="48" spans="1:10" ht="30">
+    <row r="48" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>102</v>
       </c>
@@ -2453,25 +2616,27 @@
         <v>195</v>
       </c>
       <c r="C48" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="E48" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="F48" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="D48" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="E48" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="F48" s="5" t="s">
-        <v>225</v>
-      </c>
-      <c r="G48" s="4"/>
+      <c r="G48" s="4" t="s">
+        <v>230</v>
+      </c>
       <c r="H48" t="s">
         <v>176</v>
       </c>
       <c r="I48" s="4"/>
       <c r="J48" s="4"/>
     </row>
-    <row r="49" spans="1:10" ht="30">
+    <row r="49" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>105</v>
       </c>
@@ -2479,25 +2644,27 @@
         <v>195</v>
       </c>
       <c r="C49" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="E49" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="F49" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="D49" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="E49" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="F49" s="5" t="s">
-        <v>226</v>
-      </c>
-      <c r="G49" s="4"/>
+      <c r="G49" s="4" t="s">
+        <v>230</v>
+      </c>
       <c r="H49" t="s">
         <v>176</v>
       </c>
       <c r="I49" s="4"/>
       <c r="J49" s="4"/>
     </row>
-    <row r="50" spans="1:10" ht="30">
+    <row r="50" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>107</v>
       </c>
@@ -2505,25 +2672,27 @@
         <v>194</v>
       </c>
       <c r="C50" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="E50" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="F50" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="D50" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="E50" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="F50" s="5" t="s">
-        <v>208</v>
-      </c>
-      <c r="G50" s="4"/>
+      <c r="G50" s="4" t="s">
+        <v>230</v>
+      </c>
       <c r="H50" t="s">
         <v>177</v>
       </c>
       <c r="I50" s="4"/>
       <c r="J50" s="4"/>
     </row>
-    <row r="51" spans="1:10" ht="30">
+    <row r="51" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>110</v>
       </c>
@@ -2531,25 +2700,27 @@
         <v>193</v>
       </c>
       <c r="C51" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="E51" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="F51" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="D51" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="E51" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="F51" s="5" t="s">
-        <v>207</v>
-      </c>
-      <c r="G51" s="4"/>
+      <c r="G51" s="4" t="s">
+        <v>230</v>
+      </c>
       <c r="H51" t="s">
         <v>178</v>
       </c>
       <c r="I51" s="4"/>
       <c r="J51" s="4"/>
     </row>
-    <row r="52" spans="1:10" ht="45">
+    <row r="52" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
         <v>112</v>
       </c>
@@ -2557,18 +2728,20 @@
         <v>193</v>
       </c>
       <c r="C52" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="E52" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="F52" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="D52" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="E52" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="F52" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="G52" s="4"/>
+      <c r="G52" s="4" t="s">
+        <v>230</v>
+      </c>
       <c r="H52" t="s">
         <v>179</v>
       </c>
@@ -2577,7 +2750,11 @@
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="G15" r:id="rId1" xr:uid="{8EFBC2B7-F8E1-49FB-BEF5-B4E8ABE63306}"/>
+    <hyperlink ref="G9" r:id="rId2" xr:uid="{3F99C6AE-21BD-42E5-806B-40ABB84794B8}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>